<commit_message>
removed references to avalink
</commit_message>
<xml_diff>
--- a/protected/budget.xlsx
+++ b/protected/budget.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mycamosun-my.sharepoint.com/personal/c0508083_camosun_ca/Documents/flora-communications/Project Management 291/Budget/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a8a7dff0b441a3a2/Documents/GitHub/flora-docs/protected/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="578" documentId="8_{03CFD5FA-EBE6-4EF0-8E30-58D03FFE73CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1115EE81-C2CB-4EB5-BC15-A551448FBC2E}"/>
+  <xr:revisionPtr revIDLastSave="580" documentId="8_{03CFD5FA-EBE6-4EF0-8E30-58D03FFE73CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F77ED4A-59E6-4259-BF09-607FCF6A7A09}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11520" activeTab="1" xr2:uid="{743E9BD4-5B24-43F7-BBE5-7D07A52DF72D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{743E9BD4-5B24-43F7-BBE5-7D07A52DF72D}"/>
   </bookViews>
   <sheets>
     <sheet name="Budget" sheetId="1" r:id="rId1"/>
@@ -1005,10 +1005,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1308,7 +1308,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1316,42 +1316,42 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1364,16 +1364,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1382,16 +1382,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1738,7 +1735,7 @@
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5703125" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" customWidth="1"/>
@@ -1750,7 +1747,7 @@
     <col min="10" max="11" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="38.25">
+    <row r="1" spans="1:11" ht="36" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1785,7 +1782,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -1819,7 +1816,7 @@
       </c>
       <c r="K2" s="23"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -1853,7 +1850,7 @@
       </c>
       <c r="K3" s="23"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -1887,7 +1884,7 @@
       </c>
       <c r="K4" s="23"/>
     </row>
-    <row r="5" spans="1:11" ht="12" customHeight="1">
+    <row r="5" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -1926,7 +1923,7 @@
         <v>2880</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="30">
+    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
@@ -1960,7 +1957,7 @@
       </c>
       <c r="K6" s="23"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
@@ -1994,7 +1991,7 @@
       </c>
       <c r="K7" s="23"/>
     </row>
-    <row r="8" spans="1:11" ht="30">
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
@@ -2028,7 +2025,7 @@
       </c>
       <c r="K8" s="23"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
@@ -2067,7 +2064,7 @@
         <v>13356.36</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
@@ -2101,7 +2098,7 @@
       </c>
       <c r="K10" s="23"/>
     </row>
-    <row r="11" spans="1:11" ht="30">
+    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>40</v>
       </c>
@@ -2135,7 +2132,7 @@
       </c>
       <c r="K11" s="23"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>43</v>
       </c>
@@ -2169,7 +2166,7 @@
       </c>
       <c r="K12" s="23"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>46</v>
       </c>
@@ -2203,7 +2200,7 @@
       </c>
       <c r="K13" s="23"/>
     </row>
-    <row r="14" spans="1:11" ht="30.75">
+    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>49</v>
       </c>
@@ -2237,7 +2234,7 @@
       </c>
       <c r="K14" s="23"/>
     </row>
-    <row r="15" spans="1:11" ht="30.75">
+    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>52</v>
       </c>
@@ -2276,7 +2273,7 @@
         <v>20661.520000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="30.75">
+    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>54</v>
       </c>
@@ -2315,27 +2312,25 @@
         <v>20661.520000000004</v>
       </c>
     </row>
-    <row r="17" spans="6:9">
-      <c r="F17" s="50"/>
+    <row r="17" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G17" s="47"/>
       <c r="H17" s="47"/>
       <c r="I17" s="47"/>
     </row>
-    <row r="18" spans="6:9">
-      <c r="F18" s="50"/>
+    <row r="18" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G18" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H18" s="52">
+      <c r="H18" s="50">
         <f>SUM(H2:H16)</f>
         <v>20400</v>
       </c>
     </row>
-    <row r="19" spans="6:9" ht="57.75">
-      <c r="G19" s="51" t="s">
+    <row r="19" spans="7:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="G19" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="I19" s="52">
+      <c r="I19" s="50">
         <f>SUM(I2:I16)</f>
         <v>261.52</v>
       </c>
@@ -2351,16 +2346,16 @@
   <dimension ref="A2:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
         <v>58</v>
       </c>
@@ -2371,117 +2366,112 @@
       <c r="F2" s="47"/>
       <c r="G2" s="47"/>
     </row>
-    <row r="3" spans="1:7">
-      <c r="B3" s="53"/>
-    </row>
-    <row r="4" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="51"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="53">
+      <c r="B4" s="51">
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="53">
+      <c r="B5" s="51">
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="53">
+      <c r="B6" s="51">
         <f>B15-550</f>
         <v>20111.52</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="B7" s="53"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="B8" s="53">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="51"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="51">
         <f>SUM(B4:B6)</f>
         <v>20661.52</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="B9" s="53"/>
-    </row>
-    <row r="10" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="51"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="54"/>
+      <c r="B10" s="52"/>
       <c r="C10" s="47"/>
       <c r="D10" s="47"/>
       <c r="E10" s="47"/>
       <c r="F10" s="47"/>
       <c r="G10" s="47"/>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="49"/>
-      <c r="B11" s="55"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-    </row>
-    <row r="12" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="51"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="53">
+      <c r="B12" s="51">
         <v>20400</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="53">
+      <c r="B13" s="51">
         <v>261.52</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="B14" s="53"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="B15" s="53">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="51"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="51">
         <f>SUM(B12:B13)</f>
         <v>20661.52</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="B16" s="53"/>
-    </row>
-    <row r="17" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="51"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="47"/>
-      <c r="B17" s="54"/>
+      <c r="B17" s="52"/>
       <c r="C17" s="47"/>
       <c r="D17" s="47"/>
       <c r="E17" s="47"/>
       <c r="F17" s="47"/>
       <c r="G17" s="47"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="56">
+      <c r="B18" s="53">
         <f>B8-B15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
-      <c r="B19" s="53"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="B20" s="53"/>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="51"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="51"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2496,7 +2486,7 @@
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
@@ -2509,12 +2499,12 @@
     <col min="12" max="12" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="48">
+    <row r="2" spans="1:12" ht="48" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
@@ -2543,7 +2533,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -2575,7 +2565,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -2607,7 +2597,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>17</v>
       </c>
@@ -2639,7 +2629,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
@@ -2652,7 +2642,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:12" ht="30.75">
+    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>72</v>
       </c>
@@ -2667,7 +2657,7 @@
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
     </row>
-    <row r="8" spans="1:12" ht="48">
+    <row r="8" spans="1:12" ht="48" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>0</v>
       </c>
@@ -2702,7 +2692,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -2741,7 +2731,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -2780,7 +2770,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -2819,7 +2809,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I13" t="s">
         <v>85</v>
       </c>
@@ -2828,7 +2818,7 @@
         <v>2880</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I14" s="21" t="s">
         <v>86</v>
       </c>
@@ -2838,7 +2828,7 @@
         <v>3120</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>87</v>
       </c>
@@ -2867,7 +2857,7 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.7109375" style="25" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" style="25" customWidth="1"/>
@@ -2882,17 +2872,17 @@
     <col min="11" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="21">
+    <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="24" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
         <v>92</v>
       </c>
@@ -2925,7 +2915,7 @@
       </c>
       <c r="K4" s="27"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="25">
         <v>1</v>
       </c>
@@ -2958,7 +2948,7 @@
         <v>36.99</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="25">
         <v>2</v>
       </c>
@@ -2991,7 +2981,7 @@
         <v>15.59</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D7" s="25">
         <v>15.59</v>
       </c>
@@ -3004,7 +2994,7 @@
       <c r="I7" s="32"/>
       <c r="J7" s="32"/>
     </row>
-    <row r="8" spans="1:11" ht="21">
+    <row r="8" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="H8" s="40" t="s">
         <v>107</v>
       </c>
@@ -3014,17 +3004,17 @@
         <v>52.58</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="24">
+    <row r="9" spans="1:11" ht="24" x14ac:dyDescent="0.4">
       <c r="A9" s="31" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
         <v>92</v>
       </c>
@@ -3057,7 +3047,7 @@
       </c>
       <c r="K11" s="27"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="25">
         <v>1</v>
       </c>
@@ -3089,7 +3079,7 @@
         <v>0.63700000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="25">
         <v>2</v>
       </c>
@@ -3121,7 +3111,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="25">
         <v>3</v>
       </c>
@@ -3153,7 +3143,7 @@
         <v>0.30499999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="25">
         <v>4</v>
       </c>
@@ -3185,7 +3175,7 @@
         <v>0.72599999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="25">
         <v>5</v>
       </c>
@@ -3217,7 +3207,7 @@
         <v>2.96</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="25">
         <v>6</v>
       </c>
@@ -3249,7 +3239,7 @@
         <v>0.89900000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="25">
         <v>7</v>
       </c>
@@ -3281,7 +3271,7 @@
         <v>0.14499999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="25">
         <v>8</v>
       </c>
@@ -3313,7 +3303,7 @@
         <v>7.6499999999999995</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="25">
         <v>9</v>
       </c>
@@ -3345,7 +3335,7 @@
         <v>0.31900000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="25">
         <v>10</v>
       </c>
@@ -3377,7 +3367,7 @@
         <v>0.14499999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="25">
         <v>11</v>
       </c>
@@ -3409,7 +3399,7 @@
         <v>2.5499999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="25">
         <v>12</v>
       </c>
@@ -3441,7 +3431,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="25">
         <v>13</v>
       </c>
@@ -3473,7 +3463,7 @@
         <v>0.52200000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="25">
         <v>14</v>
       </c>
@@ -3505,7 +3495,7 @@
         <v>1.19</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="25">
         <v>15</v>
       </c>
@@ -3537,7 +3527,7 @@
         <v>0.91400000000000003</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="25">
         <v>16</v>
       </c>
@@ -3569,7 +3559,7 @@
         <v>0.95700000000000007</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="25">
         <v>17</v>
       </c>
@@ -3601,7 +3591,7 @@
         <v>1.044</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="25">
         <v>18</v>
       </c>
@@ -3633,7 +3623,7 @@
         <v>2.2599999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="25">
         <v>19</v>
       </c>
@@ -3665,7 +3655,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="25">
         <v>20</v>
       </c>
@@ -3697,7 +3687,7 @@
         <v>1.74</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="25">
         <v>21</v>
       </c>
@@ -3729,7 +3719,7 @@
         <v>1.39</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="25">
         <v>22</v>
       </c>
@@ -3761,7 +3751,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="25">
         <v>23</v>
       </c>
@@ -3793,7 +3783,7 @@
         <v>10.69</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="25">
         <v>24</v>
       </c>
@@ -3825,7 +3815,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="25">
         <v>25</v>
       </c>
@@ -3857,7 +3847,7 @@
         <v>0.14499999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="25">
         <v>26</v>
       </c>
@@ -3889,7 +3879,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="25">
         <v>27</v>
       </c>
@@ -3921,7 +3911,7 @@
         <v>0.189</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="25">
         <v>28</v>
       </c>
@@ -3953,7 +3943,7 @@
         <v>0.43499999999999994</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="25">
         <v>29</v>
       </c>
@@ -3985,7 +3975,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="25">
         <v>30</v>
       </c>
@@ -4017,7 +4007,7 @@
         <v>0.14499999999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="25">
         <v>31</v>
       </c>
@@ -4049,7 +4039,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="25">
         <v>32</v>
       </c>
@@ -4081,7 +4071,7 @@
         <v>7.2499999999999995E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="25">
         <v>33</v>
       </c>
@@ -4113,7 +4103,7 @@
         <v>0.14499999999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="25">
         <v>34</v>
       </c>
@@ -4145,7 +4135,7 @@
         <v>0.14499999999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="25">
         <v>35</v>
       </c>
@@ -4177,7 +4167,7 @@
         <v>0.14499999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="25">
         <v>36</v>
       </c>
@@ -4209,7 +4199,7 @@
         <v>0.43499999999999994</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="25">
         <v>37</v>
       </c>
@@ -4241,7 +4231,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="25">
         <v>38</v>
       </c>
@@ -4273,7 +4263,7 @@
         <v>0.14499999999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="25">
         <v>39</v>
       </c>
@@ -4305,7 +4295,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="25">
         <v>40</v>
       </c>
@@ -4337,7 +4327,7 @@
         <v>0.14499999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="25">
         <v>41</v>
       </c>
@@ -4369,7 +4359,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="25">
         <v>42</v>
       </c>
@@ -4401,7 +4391,7 @@
         <v>0.60899999999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="25">
         <v>43</v>
       </c>
@@ -4433,7 +4423,7 @@
         <v>1.0230000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="25">
         <v>44</v>
       </c>
@@ -4465,7 +4455,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="25">
         <v>45</v>
       </c>
@@ -4497,7 +4487,7 @@
         <v>10.85</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="25">
         <v>46</v>
       </c>
@@ -4529,7 +4519,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="25">
         <v>47</v>
       </c>
@@ -4561,22 +4551,22 @@
         <v>9.61</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="25">
         <v>48</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="25">
         <v>49</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="25">
         <v>50</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H62" s="33" t="s">
         <v>305</v>
       </c>
@@ -4585,12 +4575,12 @@
         <v>74.551500000000019</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="36" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="25">
         <v>51</v>
       </c>
@@ -4622,7 +4612,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="25">
         <v>52</v>
       </c>
@@ -4654,7 +4644,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="25">
         <v>53</v>
       </c>
@@ -4687,7 +4677,7 @@
         <v>1.62</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H72" s="37" t="s">
         <v>317</v>
       </c>
@@ -4697,13 +4687,13 @@
         <v>3.63</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G74" s="32"/>
       <c r="H74" s="32"/>
       <c r="I74" s="32"/>
       <c r="J74" s="32"/>
     </row>
-    <row r="75" spans="1:10" ht="21">
+    <row r="75" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="H75" s="40" t="s">
         <v>318</v>
       </c>

</xml_diff>